<commit_message>
added test type flags
</commit_message>
<xml_diff>
--- a/data/processed/train/tasks.xlsx
+++ b/data/processed/train/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\hack\HSE AI Assistant hack\pocket-tutor-py\data\processed\train\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C84C10-9275-4CCE-A036-4960E269E3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9799F71B-DE3B-4961-9B13-296CFF1C10B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -631,9 +631,6 @@
 print(designer (designers, sizes, towns))</t>
   </si>
   <si>
-    <t>data = eval(open('input.txt'.read()))</t>
-  </si>
-  <si>
     <t>import os
 #data = eval(open(os.path.join(os.path.dirname(__file__), 'input.txt')).read())
 data = eval(input())
@@ -648,6 +645,9 @@
         return ([True, summa])
     return False
 print(text_check(data))</t>
+  </si>
+  <si>
+    <t>data = eval(input())</t>
   </si>
 </sst>
 </file>
@@ -1029,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1423,10 +1423,10 @@
         <v>45</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" t="s">
         <v>67</v>
-      </c>
-      <c r="E23" t="s">
-        <v>66</v>
       </c>
       <c r="F23" t="s">
         <v>56</v>

</xml_diff>